<commit_message>
update test to check on new overrides
</commit_message>
<xml_diff>
--- a/tests/test_data/test_regions_sectors.xlsx
+++ b/tests/test_data/test_regions_sectors.xlsx
@@ -522,28 +522,28 @@
         <v>32.85454545454546</v>
       </c>
       <c r="H2">
-        <v>35.07914438502674</v>
+        <v>34.58258212375859</v>
       </c>
       <c r="I2">
-        <v>36.52299465240642</v>
+        <v>34.91871657754011</v>
       </c>
       <c r="J2">
-        <v>37.76577540106952</v>
+        <v>34.90099312452253</v>
       </c>
       <c r="K2">
-        <v>38.80748663101604</v>
+        <v>34.52941176470589</v>
       </c>
       <c r="L2">
-        <v>39.64812834224599</v>
+        <v>36.01176470588235</v>
       </c>
       <c r="M2">
-        <v>40.28770053475936</v>
+        <v>37.4</v>
       </c>
       <c r="N2">
-        <v>40.72620320855615</v>
+        <v>38.69411764705882</v>
       </c>
       <c r="O2">
-        <v>40.96363636363637</v>
+        <v>39.89411764705883</v>
       </c>
       <c r="P2">
         <v>41</v>
@@ -622,28 +622,28 @@
         <v>17.45454545454546</v>
       </c>
       <c r="H4">
-        <v>18.56149732620321</v>
+        <v>18.06493506493507</v>
       </c>
       <c r="I4">
-        <v>19.24064171122994</v>
+        <v>17.63636363636364</v>
       </c>
       <c r="J4">
-        <v>19.81283422459893</v>
+        <v>16.94805194805195</v>
       </c>
       <c r="K4">
-        <v>20.27807486631016</v>
+        <v>16</v>
       </c>
       <c r="L4">
-        <v>20.63636363636364</v>
+        <v>17</v>
       </c>
       <c r="M4">
-        <v>20.88770053475936</v>
+        <v>18</v>
       </c>
       <c r="N4">
-        <v>21.03208556149733</v>
+        <v>19</v>
       </c>
       <c r="O4">
-        <v>21.06951871657754</v>
+        <v>20</v>
       </c>
       <c r="P4">
         <v>21</v>
@@ -672,28 +672,28 @@
         <v>32.85454545454546</v>
       </c>
       <c r="H5">
-        <v>35.07914438502674</v>
+        <v>34.58258212375859</v>
       </c>
       <c r="I5">
-        <v>36.52299465240642</v>
+        <v>34.91871657754011</v>
       </c>
       <c r="J5">
-        <v>37.76577540106952</v>
+        <v>34.90099312452253</v>
       </c>
       <c r="K5">
-        <v>38.80748663101604</v>
+        <v>34.52941176470589</v>
       </c>
       <c r="L5">
-        <v>39.64812834224599</v>
+        <v>36.01176470588235</v>
       </c>
       <c r="M5">
-        <v>40.28770053475936</v>
+        <v>37.4</v>
       </c>
       <c r="N5">
-        <v>40.72620320855615</v>
+        <v>38.69411764705882</v>
       </c>
       <c r="O5">
-        <v>40.96363636363637</v>
+        <v>39.89411764705883</v>
       </c>
       <c r="P5">
         <v>41</v>
@@ -772,28 +772,28 @@
         <v>17.45454545454546</v>
       </c>
       <c r="H7">
-        <v>18.56149732620321</v>
+        <v>18.06493506493507</v>
       </c>
       <c r="I7">
-        <v>19.24064171122994</v>
+        <v>17.63636363636364</v>
       </c>
       <c r="J7">
-        <v>19.81283422459893</v>
+        <v>16.94805194805195</v>
       </c>
       <c r="K7">
-        <v>20.27807486631016</v>
+        <v>16</v>
       </c>
       <c r="L7">
-        <v>20.63636363636364</v>
+        <v>17</v>
       </c>
       <c r="M7">
-        <v>20.88770053475936</v>
+        <v>18</v>
       </c>
       <c r="N7">
-        <v>21.03208556149733</v>
+        <v>19</v>
       </c>
       <c r="O7">
-        <v>21.06951871657754</v>
+        <v>20</v>
       </c>
       <c r="P7">
         <v>21</v>

</xml_diff>